<commit_message>
New analysis because of CHAOS!!!
</commit_message>
<xml_diff>
--- a/NJ/Overview.xlsx
+++ b/NJ/Overview.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="26">
   <si>
     <t>Run</t>
   </si>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
         <v>4</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F55" si="0">E3*4</f>
+        <f t="shared" ref="F3:F49" si="0">E3*4</f>
         <v>0</v>
       </c>
     </row>
@@ -1085,9 +1085,6 @@
       </c>
       <c r="H43" t="s">
         <v>10</v>
-      </c>
-      <c r="I43" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>